<commit_message>
Fixed border region station logic
</commit_message>
<xml_diff>
--- a/input/stationAddresses.xlsx
+++ b/input/stationAddresses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\thesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC0031F-06CB-4A56-BD52-00B65BC476B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0252226-E11E-4D01-8F67-3122337571C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="15585" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4B0D1EE3-07DA-4BB2-A671-24263A9F0D10}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="245">
   <si>
     <t>Acht</t>
   </si>
@@ -743,9 +743,6 @@
     <t>3199, Maasvlakte Rotterdam</t>
   </si>
   <si>
-    <t>Can switch drivers?</t>
-  </si>
-  <si>
     <t>Krefeld Gbf</t>
   </si>
   <si>
@@ -767,10 +764,13 @@
     <t>74321 Bietigheim-Bissingen, Germany</t>
   </si>
   <si>
-    <t>Netherlands, Germany</t>
-  </si>
-  <si>
-    <t>Country qualifications</t>
+    <t>Is border?</t>
+  </si>
+  <si>
+    <t>Is in border region?</t>
+  </si>
+  <si>
+    <t>Country</t>
   </si>
 </sst>
 </file>
@@ -1142,1381 +1142,1655 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C23A643-29F4-469D-948F-B38812878EAE}">
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="48.81640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="21" style="3" customWidth="1"/>
-    <col min="3" max="4" width="48.81640625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="3"/>
+    <col min="2" max="2" width="13.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.7265625" style="3" customWidth="1"/>
+    <col min="4" max="5" width="48.81640625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>141</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C2,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E2" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D2,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Achtseweg Zuid, Eindhoven</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C3,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E3" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D3,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Stationsstraat, 7607 ET Almelo</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C4,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E4" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D4,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Piet Mondriaanplein 59, 3818 GZ Amersfoort</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C5,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E5" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D5,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Stationsplein, 1012 AB Amsterdam</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C6,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E6" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D6,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Westhavenweg, 1014 BD Amsterdam</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C7,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E7" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D7,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Hornweg 32, 1044 AN  Amsterdam</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C8,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E8" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D8,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Europaweg 910, 3199 LC Maasvlakte Rotterdam</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C9,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E9" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D9,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Funkenstiege 25, 48455 Bad Bentheim, Duitsland</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D10" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C10,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E10" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D10,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Nieuwe Atelierstraat 7, Berkel-Enschot</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C11,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E11" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D11,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Halve Maan, Beverwijk</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C12,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E12" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D12,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Halve Maan, Beverwijk</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C13,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E13" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D13,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Halve Maan, Beverwijk</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B14" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="D14" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C14,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E14" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D14,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>74321 Bietigheim-Bissingen, Germany</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C15,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E15" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D15,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Botlek Rotterdam</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C16,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E16" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D16,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Botlek Rotterdam</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>228</v>
       </c>
       <c r="B17" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C17,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E17" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D17,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Botlek Rotterdam</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D18" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C18,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E18" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D18,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Bottrop, Duitsland</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C19,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E19" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D19,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Salzstraße 6, 41460 Neuss, Duitsland</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B20" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C20,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E20" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D20,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Saxion Deventer Ophaalpunt</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C21,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E21" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D21,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Saxion Deventer Ophaalpunt</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C22,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E22" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D22,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Dokweg, 3316 AD Dordrecht</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B23" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C23,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E23" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D23,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>An d. Westfalenburg 11-23, 44339 Dortmund, Duitsland</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C24,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E24" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D24,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>47055 Duisburg, Duitsland</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B25" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C25,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E25" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D25,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>47055 Duisburg, Duitsland</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B26" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C26" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C26,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E26" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D26,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Sympherstraße, 47137 Duisburg, Duitsland</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C27,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E27" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D27,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Sympherstraße, 47137 Duisburg, Duitsland</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B28" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C28" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="D28" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C28,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E28" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D28,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Coloradoweg 3199, Maasvlakte Rotterdam</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B29" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="D29" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C29,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E29" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D29,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Coloradoweg 3199, Maasvlakte Rotterdam</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C30" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C30,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E30" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D30,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Eltville Ost, Duitsland</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B31" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C31" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C31,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E31" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D31,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Bahnhofstraße 9, 46446 Emmerich am Rhein, Duitsland</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B32" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C32,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E32" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D32,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Bahnhofstraße 9, 46446 Emmerich am Rhein, Duitsland</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B33" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C33,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E33" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D33,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Maasvlakteweg 951, 3199 LZ Maasvlakte Rotterdam</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B34" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C34,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E34" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D34,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Piri Reisweg, Sevenum</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B35" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C35" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C35,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E35" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D35,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Germersheim, Duitsland</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B36" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C36" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C36,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E36" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D36,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Stationspark 14, 4461 HK Goes</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B37" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C37" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D37" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C37,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E37" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D37,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Sloterbeekstraat 1, 5912 GS Venlo</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B38" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D38" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C38,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E38" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D38,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Ruijgoordweg 100, 1047 HM Amsterdam</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B39" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C39" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D39" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C39,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E39" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D39,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Dortmuiden 5152, Amsterdam</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B40" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C40" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D40" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C40,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E40" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D40,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Aristotelesstraat, 3076 BD Rotterdam</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B41" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C41" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D41" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C41,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E41" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D41,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Bahnhofstraße 1, 41334 Nettetal, Duitsland</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B42" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C42" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D42" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C42,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E42" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D42,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Develsingel, Zwijndrecht</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B43" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C43" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D43" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C43,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E43" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D43,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Develsingel, Zwijndrecht</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B44" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C44" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D44" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C44,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E44" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D44,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Botlek Rotterdam</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B45" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D45" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C45,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E45" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D45,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Vondelingenweg 540, 3196 KK Vondelingenplaat</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B46" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D46" t="s">
         <v>57</v>
       </c>
-      <c r="D46" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C46,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E46" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D46,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>47809 Krefeld, Duitsland</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B47" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C47" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D47" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C47,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E47" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D47,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Oostelijke Parallelweg 4, Zevenbergschen Hoek</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B48" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C48" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D48" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C48,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E48" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D48,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Oggersheim, Ludwigshafen, Duitsland</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B49" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C49" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D49" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C49,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E49" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D49,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Magallanesstraat 51, 3199 LP Maasvlakte Rotterdam</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B50" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C50" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D50" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C50,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E50" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D50,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Magallanesstraat 51, 3199 LP Maasvlakte Rotterdam</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B51" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C51" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D51" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C51,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E51" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D51,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Europaweg 910, 3199 LC Maasvlakte Rotterdam</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B52" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C52" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D52" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C52,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E52" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D52,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>3199, Maasvlakte Rotterdam</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B53" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C53" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D53" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C53,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E53" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D53,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Magallanesstraat 51, 3199 LP Maasvlakte Rotterdam</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B54" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C54" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D54" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C54,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E54" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D54,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Magallanesstraat 51, 3199 LP Maasvlakte Rotterdam</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>100</v>
       </c>
       <c r="B55" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C55" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D55" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C55,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E55" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D55,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Magallanesstraat 51, 3199 LP Maasvlakte Rotterdam</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>102</v>
       </c>
       <c r="B56" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C56" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D56" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C56,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E56" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D56,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Maasvlakteweg 951, 3199 LZ Maasvlakte Rotterdam</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>104</v>
       </c>
       <c r="B57" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C57" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D57" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D57" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C57,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E57" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D57,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Magdeburg Hbf, Magdeburg, Duitsland</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B58" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C58" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D58" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C58,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E58" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D58,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Streefwaalseweg 15, 3195 KN Pernis</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B59" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C59" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D59" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C59,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E59" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D59,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Moers, Bahnhof, Moers, Duitsland</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>110</v>
       </c>
       <c r="B60" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C60" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D60" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C60,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E60" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D60,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Moers, Bahnhof, Moers, Duitsland</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B61" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C61" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D61" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C61,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E61" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D61,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Salzstraße 6, 41460 Neuss, Duitsland</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B62" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C62" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D62" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D62" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C62,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E62" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D62,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Moezelhavenweg 10, 1043 AM Amsterdam</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B63" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C63" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D63" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D63" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C63,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E63" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D63,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Westhavenweg 54-13, 1042 AL Amsterdam</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B64" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C64" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="D64" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D64" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C64,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E64" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D64,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Stationsstraat, 7573 AT Oldenzaal</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>115</v>
       </c>
       <c r="B65" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C65" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D65" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C65,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E65" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D65,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Stationsstraat, 7573 AT Oldenzaal</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>116</v>
       </c>
       <c r="B66" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C66" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D66" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C66,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E66" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D66,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Waalkade 33, 5347 KS Oss</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>117</v>
       </c>
       <c r="B67" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C67" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D67" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D67" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C67,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E67" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D67,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Opladen, Duitsland</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>118</v>
       </c>
       <c r="B68" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C68" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D68" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D68" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C68,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E68" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D68,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Waalkade 33, 5347 KS Oss</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>119</v>
       </c>
       <c r="B69" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C69" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D69" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D69" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C69,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E69" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D69,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Vondelingenweg 493, 3194 AJ Hoogvliet Rotterdam</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>120</v>
       </c>
       <c r="B70" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C70" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D70" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C70,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E70" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D70,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Fuutlaan, 5642 CV Eindhoven</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>121</v>
       </c>
       <c r="B71" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C71" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D71" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C71,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E71" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D71,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Nieuwe Atelierstraat 7, Berkel-Enschot</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B72" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C72" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D72" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D72" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C72,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E72" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D72,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Rheine, Duitsland</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B73" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C73" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D73" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D73" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C73,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E73" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D73,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Kruppstraße 12, 47229 Duisburg, Duitsland</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B74" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C74" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C74" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D74" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C74,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E74" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D74,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Bosstraat 3, 4704 RL Roosendaal</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B75" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C75" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C75" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D75" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C75,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E75" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D75,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>3199, Maasvlakte Rotterdam</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B76" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C76" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D76" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D76" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C76,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E76" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D76,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>4455 ST Nieuwdorp</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B77" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C77" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D77" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D77" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C77,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E77" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D77,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Corsicaweg 343, 1044 AB Amsterdam</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>128</v>
       </c>
       <c r="B78" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C78" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C78" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D78" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D78" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C78,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E78" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D78,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Houtbeekweg 2, 3776 LZ Stroe</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B79" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="D79" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C79,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <v>0</v>
+      </c>
+      <c r="C79" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="E79" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D79,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Arnulf-Klett-Platz 2, 70173 Stuttgart, Germany</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B80" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="D80" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C80,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <v>0</v>
+      </c>
+      <c r="C80" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="E80" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D80,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Arnulf-Klett-Platz 2, 70173 Stuttgart, Germany</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>129</v>
       </c>
       <c r="B81" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C81" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D81" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D81" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C81,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E81" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D81,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Nieuwe Atelierstraat 7, Berkel-Enschot</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B82" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C82" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C82" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D82" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D82" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C82,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E82" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D82,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Uitgeest</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B83" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C83" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="D83" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D83" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C83,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E83" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D83,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Sloterbeekstraat 1, 5912 GS Venlo</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>132</v>
       </c>
       <c r="B84" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C84" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D84" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D84" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C84,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E84" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D84,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Sloterbeekstraat 1, 5912 GS Venlo</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
         <v>133</v>
       </c>
       <c r="B85" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C85" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C85" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D85" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D85" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C85,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E85" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D85,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Dammweg, 41747 Viersen, Duitsland</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B86" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C86" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D86" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D86" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C86,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E86" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D86,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Botlek Rotterdam</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
         <v>135</v>
       </c>
       <c r="B87" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C87" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C87" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D87" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D87" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C87,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E87" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D87,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Botlek Rotterdam</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
         <v>136</v>
       </c>
       <c r="B88" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C88" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C88" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D88" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D88" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C88,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E88" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D88,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Frankrijkweg 4, 4455 TR Nieuwdorp</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B89" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C89" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C89" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D89" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D89" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C89,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E89" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D89,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Albert Plesmanweg 120, 3088 GD Rotterdam</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
         <v>138</v>
       </c>
       <c r="B90" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C90" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D90" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D90" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C90,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E90" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D90,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Stationsstraat 14, 6901 BG Zevenaar</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
         <v>139</v>
       </c>
       <c r="B91" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C91" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D91" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D91" s="3" t="str">
-        <f>_xlfn.XLOOKUP(C91,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+      <c r="E91" s="3" t="str">
+        <f>_xlfn.XLOOKUP(D91,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Overweg, 7202 AB Zutphen</v>
       </c>
     </row>
@@ -2530,13 +2804,13 @@
   <dimension ref="A1:D99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="48.81640625" customWidth="1"/>
-    <col min="3" max="3" width="29.1796875" customWidth="1"/>
+    <col min="3" max="3" width="22.6328125" customWidth="1"/>
     <col min="4" max="4" width="32.90625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2664,7 +2938,7 @@
         <v>150</v>
       </c>
       <c r="C11" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -2675,7 +2949,7 @@
         <v>151</v>
       </c>
       <c r="C12" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -2691,10 +2965,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>240</v>
+      </c>
+      <c r="B14" t="s">
         <v>241</v>
-      </c>
-      <c r="B14" t="s">
-        <v>242</v>
       </c>
       <c r="C14" t="s">
         <v>230</v>
@@ -2885,7 +3159,7 @@
         <v>165</v>
       </c>
       <c r="C30" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -3012,7 +3286,7 @@
         <v>174</v>
       </c>
       <c r="C41" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
@@ -3230,7 +3504,7 @@
         <v>190</v>
       </c>
       <c r="C60" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
@@ -3381,10 +3655,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
+        <v>236</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="C74" t="s">
         <v>230</v>
@@ -3434,7 +3708,7 @@
         <v>203</v>
       </c>
       <c r="C78" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
@@ -3511,7 +3785,7 @@
         <v>210</v>
       </c>
       <c r="C85" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Split into separate projects for algorithm and UI
</commit_message>
<xml_diff>
--- a/input/stationAddresses.xlsx
+++ b/input/stationAddresses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\thesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16B6988-F395-4C94-A1FC-64E822CEDB20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8751B1BB-6C75-40CB-B82F-E781C6667237}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="12804" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4B0D1EE3-07DA-4BB2-A671-24263A9F0D10}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="244">
   <si>
     <t>Acht</t>
   </si>
@@ -736,9 +736,6 @@
     <t>Krefeld Gbf</t>
   </si>
   <si>
-    <t>Stuttgart</t>
-  </si>
-  <si>
     <t>Is border?</t>
   </si>
   <si>
@@ -770,12 +767,6 @@
   </si>
   <si>
     <t>Houtrakpolder aansl.(Amsterdam)</t>
-  </si>
-  <si>
-    <t>Stuttgart, Germany</t>
-  </si>
-  <si>
-    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -1149,10 +1140,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C23A643-29F4-469D-948F-B38812878EAE}">
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1169,10 +1160,10 @@
         <v>139</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>234</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>235</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>223</v>
@@ -1195,7 +1186,7 @@
         <v>35</v>
       </c>
       <c r="E2" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D2,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D2,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Achtseweg Zuid, Eindhoven</v>
       </c>
     </row>
@@ -1213,7 +1204,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D3,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D3,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Stationsstraat, 7607 ET Almelo</v>
       </c>
     </row>
@@ -1231,7 +1222,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D4,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D4,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Piet Mondriaanplein 59, 3818 GZ Amersfoort</v>
       </c>
     </row>
@@ -1249,7 +1240,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D5,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D5,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Stationsplein, 1012 AB Amsterdam</v>
       </c>
     </row>
@@ -1267,7 +1258,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D6,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D6,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Westhavenweg, 1014 BD Amsterdam</v>
       </c>
     </row>
@@ -1285,7 +1276,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D7,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D7,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Hornweg 32, 1044 AN  Amsterdam</v>
       </c>
     </row>
@@ -1303,7 +1294,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D8,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D8,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Europaweg 910, 3199 LC Maasvlakte Rotterdam</v>
       </c>
     </row>
@@ -1321,7 +1312,7 @@
         <v>9</v>
       </c>
       <c r="E9" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D9,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D9,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Funkenstiege 25, 48455 Bad Bentheim, Duitsland</v>
       </c>
     </row>
@@ -1339,7 +1330,7 @@
         <v>89</v>
       </c>
       <c r="E10" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D10,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D10,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Nieuwe Atelierstraat 7, Berkel-Enschot</v>
       </c>
     </row>
@@ -1357,7 +1348,7 @@
         <v>13</v>
       </c>
       <c r="E11" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D11,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D11,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Halve Maan, Beverwijk</v>
       </c>
     </row>
@@ -1375,7 +1366,7 @@
         <v>13</v>
       </c>
       <c r="E12" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D12,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D12,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Halve Maan, Beverwijk</v>
       </c>
     </row>
@@ -1393,7 +1384,7 @@
         <v>13</v>
       </c>
       <c r="E13" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D13,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D13,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Halve Maan, Beverwijk</v>
       </c>
     </row>
@@ -1411,7 +1402,7 @@
         <v>19</v>
       </c>
       <c r="E14" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D14,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D14,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Botlek Rotterdam</v>
       </c>
     </row>
@@ -1429,7 +1420,7 @@
         <v>19</v>
       </c>
       <c r="E15" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D15,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D15,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Botlek Rotterdam</v>
       </c>
     </row>
@@ -1447,7 +1438,7 @@
         <v>19</v>
       </c>
       <c r="E16" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D16,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D16,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Botlek Rotterdam</v>
       </c>
     </row>
@@ -1465,7 +1456,7 @@
         <v>215</v>
       </c>
       <c r="E17" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D17,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D17,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Bottrop, Duitsland</v>
       </c>
     </row>
@@ -1483,7 +1474,7 @@
         <v>67</v>
       </c>
       <c r="E18" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D18,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D18,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Salzstraße 6, 41460 Neuss, Duitsland</v>
       </c>
     </row>
@@ -1501,7 +1492,7 @@
         <v>23</v>
       </c>
       <c r="E19" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D19,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D19,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Saxion Deventer Ophaalpunt</v>
       </c>
     </row>
@@ -1519,7 +1510,7 @@
         <v>23</v>
       </c>
       <c r="E20" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D20,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D20,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Saxion Deventer Ophaalpunt</v>
       </c>
     </row>
@@ -1537,7 +1528,7 @@
         <v>25</v>
       </c>
       <c r="E21" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D21,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D21,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Dokweg, 3316 AD Dordrecht</v>
       </c>
     </row>
@@ -1555,7 +1546,7 @@
         <v>27</v>
       </c>
       <c r="E22" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D22,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D22,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>An d. Westfalenburg 11-23, 44339 Dortmund, Duitsland</v>
       </c>
     </row>
@@ -1573,7 +1564,7 @@
         <v>31</v>
       </c>
       <c r="E23" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D23,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D23,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>47055 Duisburg, Duitsland</v>
       </c>
     </row>
@@ -1591,7 +1582,7 @@
         <v>31</v>
       </c>
       <c r="E24" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D24,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D24,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>47055 Duisburg, Duitsland</v>
       </c>
     </row>
@@ -1609,7 +1600,7 @@
         <v>29</v>
       </c>
       <c r="E25" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D25,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D25,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Sympherstraße, 47137 Duisburg, Duitsland</v>
       </c>
     </row>
@@ -1627,7 +1618,7 @@
         <v>29</v>
       </c>
       <c r="E26" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D26,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D26,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Sympherstraße, 47137 Duisburg, Duitsland</v>
       </c>
     </row>
@@ -1645,7 +1636,7 @@
         <v>229</v>
       </c>
       <c r="E27" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D27,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D27,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Coloradoweg 3199, Maasvlakte Rotterdam</v>
       </c>
     </row>
@@ -1663,7 +1654,7 @@
         <v>229</v>
       </c>
       <c r="E28" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D28,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D28,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Coloradoweg 3199, Maasvlakte Rotterdam</v>
       </c>
     </row>
@@ -1681,7 +1672,7 @@
         <v>51</v>
       </c>
       <c r="E29" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D29,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D29,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Eltville Ost, Duitsland</v>
       </c>
     </row>
@@ -1699,7 +1690,7 @@
         <v>37</v>
       </c>
       <c r="E30" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D30,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D30,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Bahnhofstraße 9, 46446 Emmerich am Rhein, Duitsland</v>
       </c>
     </row>
@@ -1717,7 +1708,7 @@
         <v>37</v>
       </c>
       <c r="E31" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D31,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D31,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Bahnhofstraße 9, 46446 Emmerich am Rhein, Duitsland</v>
       </c>
     </row>
@@ -1735,13 +1726,13 @@
         <v>57</v>
       </c>
       <c r="E32" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D32,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D32,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Maasvlakteweg 951, 3199 LZ Maasvlakte Rotterdam</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B33" s="6" t="b">
         <v>0</v>
@@ -1753,7 +1744,7 @@
         <v>39</v>
       </c>
       <c r="E33" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D33,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D33,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Moezelweg 100, 3198 LS Europoort Rotterdam</v>
       </c>
     </row>
@@ -1771,7 +1762,7 @@
         <v>41</v>
       </c>
       <c r="E34" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D34,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D34,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Piri Reisweg, Sevenum</v>
       </c>
     </row>
@@ -1789,7 +1780,7 @@
         <v>62</v>
       </c>
       <c r="E35" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D35,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D35,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Stationspark 14, 4461 HK Goes</v>
       </c>
     </row>
@@ -1807,7 +1798,7 @@
         <v>95</v>
       </c>
       <c r="E36" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D36,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D36,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Sloterbeekstraat 1, 5912 GS Venlo</v>
       </c>
     </row>
@@ -1825,7 +1816,7 @@
         <v>66</v>
       </c>
       <c r="E37" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D37,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D37,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Ruijgoordweg 100, 1047 HM Amsterdam</v>
       </c>
     </row>
@@ -1840,16 +1831,16 @@
         <v>0</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E38" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D38,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D38,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Dortmuiden 5152, Amsterdam</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B39" s="6" t="b">
         <v>0</v>
@@ -1858,10 +1849,10 @@
         <v>0</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E39" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D39,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D39,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Dortmuiden 5152, Amsterdam</v>
       </c>
     </row>
@@ -1879,7 +1870,7 @@
         <v>48</v>
       </c>
       <c r="E40" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D40,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D40,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Aristotelesstraat, 3076 BD Rotterdam</v>
       </c>
     </row>
@@ -1897,7 +1888,7 @@
         <v>50</v>
       </c>
       <c r="E41" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D41,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D41,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Bahnhofstraße 1, 41334 Nettetal, Duitsland</v>
       </c>
     </row>
@@ -1915,7 +1906,7 @@
         <v>52</v>
       </c>
       <c r="E42" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D42,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D42,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Develsingel, Zwijndrecht</v>
       </c>
     </row>
@@ -1933,7 +1924,7 @@
         <v>52</v>
       </c>
       <c r="E43" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D43,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D43,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Develsingel, Zwijndrecht</v>
       </c>
     </row>
@@ -1951,7 +1942,7 @@
         <v>19</v>
       </c>
       <c r="E44" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D44,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D44,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Botlek Rotterdam</v>
       </c>
     </row>
@@ -1969,7 +1960,7 @@
         <v>80</v>
       </c>
       <c r="E45" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D45,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D45,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Vondelingenweg 540, 3196 KK Vondelingenplaat</v>
       </c>
     </row>
@@ -1987,7 +1978,7 @@
         <v>56</v>
       </c>
       <c r="E46" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D46,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D46,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>47809 Krefeld, Duitsland</v>
       </c>
     </row>
@@ -2005,7 +1996,7 @@
         <v>58</v>
       </c>
       <c r="E47" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D47,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D47,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Oostelijke Parallelweg 4, Zevenbergschen Hoek</v>
       </c>
     </row>
@@ -2023,7 +2014,7 @@
         <v>84</v>
       </c>
       <c r="E48" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D48,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D48,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Oggersheim, Ludwigshafen, Duitsland</v>
       </c>
     </row>
@@ -2041,7 +2032,7 @@
         <v>61</v>
       </c>
       <c r="E49" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D49,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D49,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Magallanesstraat 51, 3199 LP Maasvlakte Rotterdam</v>
       </c>
     </row>
@@ -2059,7 +2050,7 @@
         <v>61</v>
       </c>
       <c r="E50" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D50,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D50,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Magallanesstraat 51, 3199 LP Maasvlakte Rotterdam</v>
       </c>
     </row>
@@ -2077,7 +2068,7 @@
         <v>12</v>
       </c>
       <c r="E51" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D51,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D51,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Europaweg 910, 3199 LC Maasvlakte Rotterdam</v>
       </c>
     </row>
@@ -2095,7 +2086,7 @@
         <v>123</v>
       </c>
       <c r="E52" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D52,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D52,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>3199, Maasvlakte Rotterdam</v>
       </c>
     </row>
@@ -2113,7 +2104,7 @@
         <v>61</v>
       </c>
       <c r="E53" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D53,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D53,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Magallanesstraat 51, 3199 LP Maasvlakte Rotterdam</v>
       </c>
     </row>
@@ -2131,7 +2122,7 @@
         <v>61</v>
       </c>
       <c r="E54" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D54,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D54,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Magallanesstraat 51, 3199 LP Maasvlakte Rotterdam</v>
       </c>
     </row>
@@ -2149,7 +2140,7 @@
         <v>61</v>
       </c>
       <c r="E55" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D55,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D55,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Magallanesstraat 51, 3199 LP Maasvlakte Rotterdam</v>
       </c>
     </row>
@@ -2167,7 +2158,7 @@
         <v>57</v>
       </c>
       <c r="E56" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D56,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D56,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Maasvlakteweg 951, 3199 LZ Maasvlakte Rotterdam</v>
       </c>
     </row>
@@ -2185,7 +2176,7 @@
         <v>102</v>
       </c>
       <c r="E57" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D57,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D57,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Magdeburg Hbf, Magdeburg, Duitsland</v>
       </c>
     </row>
@@ -2203,7 +2194,7 @@
         <v>104</v>
       </c>
       <c r="E58" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D58,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D58,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Streefwaalseweg 15, 3195 KN Pernis</v>
       </c>
     </row>
@@ -2221,7 +2212,7 @@
         <v>106</v>
       </c>
       <c r="E59" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D59,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D59,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Moers, Bahnhof, Moers, Duitsland</v>
       </c>
     </row>
@@ -2239,7 +2230,7 @@
         <v>106</v>
       </c>
       <c r="E60" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D60,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D60,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Moers, Bahnhof, Moers, Duitsland</v>
       </c>
     </row>
@@ -2257,7 +2248,7 @@
         <v>67</v>
       </c>
       <c r="E61" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D61,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D61,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Salzstraße 6, 41460 Neuss, Duitsland</v>
       </c>
     </row>
@@ -2275,7 +2266,7 @@
         <v>138</v>
       </c>
       <c r="E62" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D62,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D62,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Moezelhavenweg 10, 1043 AM Amsterdam</v>
       </c>
     </row>
@@ -2293,7 +2284,7 @@
         <v>111</v>
       </c>
       <c r="E63" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D63,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D63,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Westhavenweg 54-13, 1042 AL Amsterdam</v>
       </c>
     </row>
@@ -2311,7 +2302,7 @@
         <v>73</v>
       </c>
       <c r="E64" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D64,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D64,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Stationsstraat, 7573 AT Oldenzaal</v>
       </c>
     </row>
@@ -2329,7 +2320,7 @@
         <v>73</v>
       </c>
       <c r="E65" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D65,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D65,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Stationsstraat, 7573 AT Oldenzaal</v>
       </c>
     </row>
@@ -2347,7 +2338,7 @@
         <v>79</v>
       </c>
       <c r="E66" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D66,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D66,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Waalkade 33, 5347 KS Oss</v>
       </c>
     </row>
@@ -2365,7 +2356,7 @@
         <v>115</v>
       </c>
       <c r="E67" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D67,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D67,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Opladen, Duitsland</v>
       </c>
     </row>
@@ -2383,7 +2374,7 @@
         <v>79</v>
       </c>
       <c r="E68" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D68,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D68,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Waalkade 33, 5347 KS Oss</v>
       </c>
     </row>
@@ -2401,7 +2392,7 @@
         <v>81</v>
       </c>
       <c r="E69" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D69,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D69,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Vondelingenweg 493, 3194 AJ Hoogvliet Rotterdam</v>
       </c>
     </row>
@@ -2419,7 +2410,7 @@
         <v>33</v>
       </c>
       <c r="E70" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D70,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D70,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Fuutlaan, 5642 CV Eindhoven</v>
       </c>
     </row>
@@ -2437,7 +2428,7 @@
         <v>89</v>
       </c>
       <c r="E71" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D71,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D71,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Nieuwe Atelierstraat 7, Berkel-Enschot</v>
       </c>
     </row>
@@ -2455,7 +2446,7 @@
         <v>120</v>
       </c>
       <c r="E72" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D72,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D72,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Rheine, Duitsland</v>
       </c>
     </row>
@@ -2473,7 +2464,7 @@
         <v>83</v>
       </c>
       <c r="E73" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D73,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D73,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Kruppstraße 12, 47229 Duisburg, Duitsland</v>
       </c>
     </row>
@@ -2491,7 +2482,7 @@
         <v>85</v>
       </c>
       <c r="E74" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D74,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D74,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Bosstraat 3, 4704 RL Roosendaal</v>
       </c>
     </row>
@@ -2509,13 +2500,13 @@
         <v>123</v>
       </c>
       <c r="E75" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D75,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D75,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>3199, Maasvlakte Rotterdam</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B76" s="6" t="b">
         <v>0</v>
@@ -2524,10 +2515,10 @@
         <v>0</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E76" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D76,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D76,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>'s-Hertogenbosch</v>
       </c>
     </row>
@@ -2545,7 +2536,7 @@
         <v>124</v>
       </c>
       <c r="E77" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D77,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D77,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>4455 ST Nieuwdorp</v>
       </c>
     </row>
@@ -2563,13 +2554,13 @@
         <v>125</v>
       </c>
       <c r="E78" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D78,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D78,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Corsicaweg 343, 1044 AB Amsterdam</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B79" s="6" t="b">
         <v>0</v>
@@ -2578,10 +2569,10 @@
         <v>0</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E79" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D79,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D79,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Den Hamweg 55, 3089 KK Rotterdam</v>
       </c>
     </row>
@@ -2599,13 +2590,13 @@
         <v>126</v>
       </c>
       <c r="E80" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D80,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D80,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Houtbeekweg 2, 3776 LZ Stroe</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
-        <v>233</v>
+        <v>127</v>
       </c>
       <c r="B81" s="6" t="b">
         <v>0</v>
@@ -2613,17 +2604,17 @@
       <c r="C81" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="D81" s="4" t="s">
-        <v>233</v>
+      <c r="D81" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="E81" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D81,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
-        <v>Stuttgart, Germany</v>
+        <f>_xlfn.XLOOKUP(D81,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <v>Nieuwe Atelierstraat 7, Berkel-Enschot</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
-        <v>127</v>
+        <v>236</v>
       </c>
       <c r="B82" s="6" t="b">
         <v>0</v>
@@ -2635,13 +2626,13 @@
         <v>89</v>
       </c>
       <c r="E82" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D82,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D82,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Nieuwe Atelierstraat 7, Berkel-Enschot</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
-        <v>237</v>
+        <v>128</v>
       </c>
       <c r="B83" s="6" t="b">
         <v>0</v>
@@ -2650,37 +2641,37 @@
         <v>0</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E83" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D83,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
-        <v>Nieuwe Atelierstraat 7, Berkel-Enschot</v>
+        <f>_xlfn.XLOOKUP(D83,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <v>Uitgeest</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B84" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C84" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E84" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D84,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
-        <v>Uitgeest</v>
+        <f>_xlfn.XLOOKUP(D84,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <v>Sloterbeekstraat 1, 5912 GS Venlo</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B85" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C85" s="6" t="b">
         <v>1</v>
@@ -2689,31 +2680,31 @@
         <v>95</v>
       </c>
       <c r="E85" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D85,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D85,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Sloterbeekstraat 1, 5912 GS Venlo</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B86" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C86" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E86" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D86,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
-        <v>Sloterbeekstraat 1, 5912 GS Venlo</v>
+        <f>_xlfn.XLOOKUP(D86,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <v>Dammweg, 41747 Viersen, Duitsland</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B87" s="6" t="b">
         <v>0</v>
@@ -2722,16 +2713,16 @@
         <v>0</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="E87" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D87,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
-        <v>Dammweg, 41747 Viersen, Duitsland</v>
+        <f>_xlfn.XLOOKUP(D87,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <v>Botlek Rotterdam</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B88" s="6" t="b">
         <v>0</v>
@@ -2743,13 +2734,13 @@
         <v>19</v>
       </c>
       <c r="E88" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D88,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D88,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Botlek Rotterdam</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B89" s="6" t="b">
         <v>0</v>
@@ -2757,17 +2748,17 @@
       <c r="C89" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="D89" s="3" t="s">
-        <v>19</v>
+      <c r="D89" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="E89" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D89,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
-        <v>Botlek Rotterdam</v>
+        <f>_xlfn.XLOOKUP(D89,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <v>Frankrijkweg 4, 4455 TR Nieuwdorp</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B90" s="6" t="b">
         <v>0</v>
@@ -2775,65 +2766,47 @@
       <c r="C90" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="D90" s="4" t="s">
-        <v>134</v>
+      <c r="D90" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="E90" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D90,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
-        <v>Frankrijkweg 4, 4455 TR Nieuwdorp</v>
+        <f>_xlfn.XLOOKUP(D90,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <v>Albert Plesmanweg 120, 3088 GD Rotterdam</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B91" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C91" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>101</v>
+        <v>1</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>136</v>
       </c>
       <c r="E91" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D91,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
-        <v>Albert Plesmanweg 120, 3088 GD Rotterdam</v>
+        <f>_xlfn.XLOOKUP(D91,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <v>Stationsstraat 14, 6901 BG Zevenaar</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B92" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C92" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>136</v>
+        <v>0</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="E92" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D92,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
-        <v>Stationsstraat 14, 6901 BG Zevenaar</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A93" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B93" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C93" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E93" s="3" t="str">
-        <f>_xlfn.XLOOKUP(D93,'Station addresses'!$A$2:$A$1013,'Station addresses'!$B$2:$B$1013,"STATION NOT FOUND IN ADDRESS LIST")</f>
+        <f>_xlfn.XLOOKUP(D92,'Station addresses'!$A$2:$A$1012,'Station addresses'!$B$2:$B$1012,"STATION NOT FOUND IN ADDRESS LIST")</f>
         <v>Overweg, 7202 AB Zutphen</v>
       </c>
     </row>
@@ -2844,10 +2817,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D40E918-4E91-4C95-B234-1F9922AFEF3D}">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+      <selection activeCell="A74" sqref="A74:XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2865,7 +2838,7 @@
         <v>210</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>216</v>
@@ -2997,10 +2970,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>239</v>
+      </c>
+      <c r="B13" t="s">
         <v>240</v>
-      </c>
-      <c r="B13" t="s">
-        <v>241</v>
       </c>
       <c r="C13" t="s">
         <v>226</v>
@@ -3287,7 +3260,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B38" t="s">
         <v>170</v>
@@ -3640,10 +3613,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C69" t="s">
         <v>226</v>
@@ -3698,24 +3671,21 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>233</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>245</v>
+        <v>89</v>
+      </c>
+      <c r="B74" t="s">
+        <v>199</v>
       </c>
       <c r="C74" t="s">
-        <v>227</v>
-      </c>
-      <c r="D74" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B75" t="s">
-        <v>199</v>
+        <v>128</v>
       </c>
       <c r="C75" t="s">
         <v>226</v>
@@ -3723,10 +3693,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B76" t="s">
-        <v>128</v>
+        <v>200</v>
       </c>
       <c r="C76" t="s">
         <v>226</v>
@@ -3734,10 +3704,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B77" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C77" t="s">
         <v>226</v>
@@ -3745,32 +3715,32 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B78" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C78" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B79" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C79" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="B80" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C80" t="s">
         <v>226</v>
@@ -3778,10 +3748,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="B81" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C81" t="s">
         <v>226</v>
@@ -3789,10 +3759,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B82" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C82" t="s">
         <v>226</v>
@@ -3800,10 +3770,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B83" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C83" t="s">
         <v>226</v>
@@ -3811,10 +3781,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>105</v>
+        <v>136</v>
       </c>
       <c r="B84" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C84" t="s">
         <v>226</v>
@@ -3822,25 +3792,18 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="B85" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C85" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>107</v>
-      </c>
-      <c r="B86" t="s">
-        <v>209</v>
-      </c>
-      <c r="C86" t="s">
-        <v>226</v>
-      </c>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B87" s="2"/>
@@ -3850,17 +3813,13 @@
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-    </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>